<commit_message>
character code doc update.
</commit_message>
<xml_diff>
--- a/doc/super-duper-display-image.xlsx
+++ b/doc/super-duper-display-image.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\daisuke\nes\super-duper-nes\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motooka\Documents\001-proj\970.moto-proj\super-duper-nes\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18015" windowHeight="8805" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18015" windowHeight="8805" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="top page" sheetId="2" r:id="rId1"/>
@@ -19,9 +19,10 @@
     <sheet name="disp map" sheetId="9" r:id="rId5"/>
     <sheet name="shell" sheetId="10" r:id="rId6"/>
     <sheet name="ascii" sheetId="4" r:id="rId7"/>
-    <sheet name="io port" sheetId="5" r:id="rId8"/>
+    <sheet name="chrrom" sheetId="11" r:id="rId8"/>
+    <sheet name="io port" sheetId="5" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="298">
   <si>
     <t>文</t>
   </si>
@@ -924,24 +925,27 @@
   </si>
   <si>
     <t>4. 読み込んだ値のbit0が0なら入力無し、1なら入力ありと言う事になる。</t>
+  </si>
+  <si>
+    <t>ascii '0' (0x30) is placed at 0x8310.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1012,7 +1016,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1641,22 +1645,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1691,7 +1695,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1749,7 +1753,7 @@
         <xdr:cNvPr id="3" name="Rounded Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1883,7 +1887,7 @@
         <xdr:cNvPr id="5" name="Rectangle 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1946,7 +1950,7 @@
         <xdr:cNvPr id="4" name="Rounded Rectangle 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2086,7 +2090,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2145,7 +2149,7 @@
         <xdr:cNvPr id="3" name="Rounded Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2238,7 +2242,7 @@
         <xdr:cNvPr id="4" name="Rounded Rectangle 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2336,7 +2340,7 @@
         <xdr:cNvPr id="5" name="Rounded Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2406,7 +2410,7 @@
         <xdr:cNvPr id="6" name="Rounded Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2486,7 +2490,7 @@
         <xdr:cNvPr id="8" name="Rounded Rectangle 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2546,7 +2550,7 @@
         <xdr:cNvPr id="9" name="Rounded Rectangular Callout 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2623,7 +2627,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2682,7 +2686,7 @@
         <xdr:cNvPr id="3" name="Rounded Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2771,7 +2775,7 @@
         <xdr:cNvPr id="4" name="Rounded Rectangle 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2844,7 +2848,7 @@
         <xdr:cNvPr id="5" name="Rounded Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2914,7 +2918,7 @@
         <xdr:cNvPr id="6" name="Rounded Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2979,7 +2983,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3040,7 +3044,7 @@
         <xdr:cNvPr id="10" name="Rounded Rectangle 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3119,7 +3123,7 @@
         <xdr:cNvPr id="11" name="Rounded Rectangle 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3187,7 +3191,7 @@
         <xdr:cNvPr id="13" name="Rounded Rectangle 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3263,7 +3267,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3322,7 +3326,7 @@
         <xdr:cNvPr id="7" name="Rounded Rectangle 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3382,7 +3386,7 @@
         <xdr:cNvPr id="8" name="Rounded Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3454,7 +3458,7 @@
         <xdr:cNvPr id="10" name="Rounded Rectangle 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3546,7 +3550,7 @@
         <xdr:cNvPr id="11" name="Rounded Rectangle 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3619,7 +3623,7 @@
         <xdr:cNvPr id="5" name="Rounded Rectangle 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3772,7 +3776,7 @@
         <xdr:cNvPr id="2" name="Rounded Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3956,7 +3960,7 @@
         <xdr:cNvPr id="3" name="Rounded Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4140,7 +4144,7 @@
         <xdr:cNvPr id="4" name="Rounded Rectangle 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4262,7 +4266,7 @@
         <xdr:cNvPr id="2" name="Rounded Rectangle 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23D2AF78-8443-4B76-8335-B99CC8FB1242}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{23D2AF78-8443-4B76-8335-B99CC8FB1242}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4415,7 +4419,7 @@
         <xdr:cNvPr id="4" name="Rounded Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86EA46A8-D46B-483F-91EB-012B372AE11B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{86EA46A8-D46B-483F-91EB-012B372AE11B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4642,7 +4646,7 @@
         <xdr:cNvPr id="5" name="Rounded Rectangle 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B769B88A-DE40-483C-98A8-F96253B2CCEB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B769B88A-DE40-483C-98A8-F96253B2CCEB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4759,7 +4763,7 @@
         <xdr:cNvPr id="6" name="Rounded Rectangle 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{094F8DA8-D9D4-4E4D-9218-B8A075169A1E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{094F8DA8-D9D4-4E4D-9218-B8A075169A1E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4811,6 +4815,545 @@
             </a:rPr>
             <a:t>| abc</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>551695</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>8952</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6038095" cy="4580952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect r="44946" b="-1260"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6572250" y="85724"/>
+          <a:ext cx="3324225" cy="4638675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rounded Rectangle 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6496050" y="4429125"/>
+          <a:ext cx="819150" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangular Callout 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10201275" y="1085850"/>
+          <a:ext cx="1238250" cy="733425"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -323070"/>
+            <a:gd name="adj2" fmla="val -69257"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>'0' is ascii 0x30</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangular Callout 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5934075" y="4972050"/>
+          <a:ext cx="2076450" cy="1009650"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -424"/>
+            <a:gd name="adj2" fmla="val -85613"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>.nes file header: 0x10</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>.nes 0x0010</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> - 0x8010 : prg rom</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>.nes </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>0x8010 - 0x10010 : chr rom</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>552449</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rounded Rectangle 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6648449" y="1571625"/>
+          <a:ext cx="2162175" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:srcRect r="49678" b="-2507"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11715750" y="295274"/>
+          <a:ext cx="3038475" cy="4695825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangular Callout 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13496925" y="1371600"/>
+          <a:ext cx="1238250" cy="733425"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -169993"/>
+            <a:gd name="adj2" fmla="val -71854"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Drawing</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> object is chr code 0x8X</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rounded Rectangle 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11658600" y="4667250"/>
+          <a:ext cx="819150" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -5081,16 +5624,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AE11" sqref="AE11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="27" spans="16:16" x14ac:dyDescent="0.15">
+    <row r="27" spans="16:16">
       <c r="P27" t="s">
         <v>248</v>
       </c>
@@ -5103,21 +5646,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C14:R20"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="3:18">
       <c r="C14" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="16" spans="3:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="3:18">
       <c r="C16" s="53"/>
       <c r="D16" s="53"/>
       <c r="E16" s="54" t="s">
@@ -5161,7 +5704,7 @@
       </c>
       <c r="R16" s="53"/>
     </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="3:18">
       <c r="C17" s="53"/>
       <c r="D17" s="53"/>
       <c r="E17" s="54" t="s">
@@ -5205,7 +5748,7 @@
       </c>
       <c r="R17" s="53"/>
     </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="3:18">
       <c r="C18" s="53"/>
       <c r="D18" s="53"/>
       <c r="E18" s="54"/>
@@ -5247,7 +5790,7 @@
       </c>
       <c r="R18" s="78"/>
     </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.15">
+    <row r="19" spans="3:18">
       <c r="C19" s="77" t="s">
         <v>250</v>
       </c>
@@ -5287,7 +5830,7 @@
       <c r="Q19" s="54"/>
       <c r="R19" s="53"/>
     </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.15">
+    <row r="20" spans="3:18">
       <c r="C20" s="53"/>
       <c r="D20" s="53"/>
       <c r="E20" s="53"/>
@@ -5320,18 +5863,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C14:Q20"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AI26" sqref="AI26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="14" spans="5:17" s="56" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="5:17" s="56" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="5:17" s="56" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="5:17" s="56" customFormat="1"/>
+    <row r="15" spans="5:17" s="56" customFormat="1"/>
+    <row r="16" spans="5:17" s="56" customFormat="1">
       <c r="E16" s="57"/>
       <c r="F16" s="57"/>
       <c r="G16" s="57"/>
@@ -5346,7 +5889,7 @@
       <c r="P16" s="58"/>
       <c r="Q16" s="58"/>
     </row>
-    <row r="17" spans="3:17" s="56" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="3:17" s="56" customFormat="1">
       <c r="E17" s="57"/>
       <c r="F17" s="57"/>
       <c r="G17" s="57"/>
@@ -5361,7 +5904,7 @@
       <c r="P17" s="57"/>
       <c r="Q17" s="57"/>
     </row>
-    <row r="18" spans="3:17" s="56" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="3:17" s="56" customFormat="1">
       <c r="E18" s="57"/>
       <c r="F18" s="57"/>
       <c r="G18" s="57"/>
@@ -5376,7 +5919,7 @@
       <c r="P18" s="58"/>
       <c r="Q18" s="57"/>
     </row>
-    <row r="19" spans="3:17" s="56" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="3:17" s="56" customFormat="1">
       <c r="C19" s="80"/>
       <c r="D19" s="80"/>
       <c r="E19" s="57"/>
@@ -5393,7 +5936,7 @@
       <c r="P19" s="57"/>
       <c r="Q19" s="57"/>
     </row>
-    <row r="20" spans="3:17" s="56" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="3:17" s="56" customFormat="1">
       <c r="I20" s="80"/>
       <c r="J20" s="80"/>
       <c r="K20" s="80"/>
@@ -5410,16 +5953,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C16:R20"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AA17" sqref="AA17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="16" spans="3:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="3:18">
       <c r="C16" s="53"/>
       <c r="D16" s="53"/>
       <c r="E16" s="54" t="s">
@@ -5463,7 +6006,7 @@
       </c>
       <c r="R16" s="53"/>
     </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="3:18">
       <c r="C17" s="53"/>
       <c r="D17" s="53"/>
       <c r="E17" s="54" t="s">
@@ -5507,7 +6050,7 @@
       </c>
       <c r="R17" s="53"/>
     </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="3:18">
       <c r="C18" s="53"/>
       <c r="D18" s="53"/>
       <c r="E18" s="54"/>
@@ -5549,7 +6092,7 @@
       </c>
       <c r="R18" s="78"/>
     </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.15">
+    <row r="19" spans="3:18">
       <c r="C19" s="77" t="s">
         <v>250</v>
       </c>
@@ -5589,7 +6132,7 @@
       <c r="Q19" s="54"/>
       <c r="R19" s="53"/>
     </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.15">
+    <row r="20" spans="3:18">
       <c r="C20" s="53"/>
       <c r="D20" s="53"/>
       <c r="E20" s="53"/>
@@ -5622,7 +6165,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BP31"/>
   <sheetViews>
     <sheetView topLeftCell="AJ1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -5630,16 +6173,16 @@
       <selection activeCell="AJ1" sqref="AJ1"/>
       <selection pane="topRight" activeCell="AK1" sqref="AK1"/>
       <selection pane="bottomLeft" activeCell="AJ2" sqref="AJ2"/>
-      <selection pane="bottomRight" activeCell="AO15" sqref="AO15"/>
+      <selection pane="bottomRight" activeCell="BS11" sqref="BS11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="4.85546875" defaultRowHeight="27" customHeight="1"/>
   <cols>
     <col min="1" max="33" width="0" hidden="1" customWidth="1"/>
-    <col min="36" max="68" width="4.875" style="59"/>
+    <col min="36" max="68" width="4.85546875" style="59"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:68" ht="27" customHeight="1" thickBot="1">
       <c r="B1">
         <v>0</v>
       </c>
@@ -5833,7 +6376,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:68" ht="27" customHeight="1">
       <c r="A2">
         <v>0</v>
       </c>
@@ -6096,7 +6639,7 @@
         <v>201F</v>
       </c>
     </row>
-    <row r="3" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:68" ht="27" customHeight="1">
       <c r="A3">
         <v>1</v>
       </c>
@@ -6360,7 +6903,7 @@
         <v>203F</v>
       </c>
     </row>
-    <row r="4" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:68" ht="27" customHeight="1">
       <c r="A4">
         <v>2</v>
       </c>
@@ -6624,7 +7167,7 @@
         <v>205F</v>
       </c>
     </row>
-    <row r="5" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:68" ht="27" customHeight="1">
       <c r="A5">
         <v>3</v>
       </c>
@@ -6888,7 +7431,7 @@
         <v>207F</v>
       </c>
     </row>
-    <row r="6" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:68" ht="27" customHeight="1">
       <c r="A6">
         <v>4</v>
       </c>
@@ -7152,7 +7695,7 @@
         <v>209F</v>
       </c>
     </row>
-    <row r="7" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:68" ht="27" customHeight="1">
       <c r="A7">
         <v>5</v>
       </c>
@@ -7416,7 +7959,7 @@
         <v>20BF</v>
       </c>
     </row>
-    <row r="8" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:68" ht="27" customHeight="1">
       <c r="A8">
         <v>6</v>
       </c>
@@ -7680,7 +8223,7 @@
         <v>20DF</v>
       </c>
     </row>
-    <row r="9" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:68" ht="27" customHeight="1">
       <c r="A9">
         <v>7</v>
       </c>
@@ -7944,7 +8487,7 @@
         <v>20FF</v>
       </c>
     </row>
-    <row r="10" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:68" ht="27" customHeight="1">
       <c r="A10">
         <v>8</v>
       </c>
@@ -8208,7 +8751,7 @@
         <v>211F</v>
       </c>
     </row>
-    <row r="11" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:68" ht="27" customHeight="1">
       <c r="A11">
         <v>9</v>
       </c>
@@ -8472,7 +9015,7 @@
         <v>213F</v>
       </c>
     </row>
-    <row r="12" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:68" ht="27" customHeight="1">
       <c r="A12">
         <v>10</v>
       </c>
@@ -8736,7 +9279,7 @@
         <v>215F</v>
       </c>
     </row>
-    <row r="13" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:68" ht="27" customHeight="1">
       <c r="A13">
         <v>11</v>
       </c>
@@ -9000,7 +9543,7 @@
         <v>217F</v>
       </c>
     </row>
-    <row r="14" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:68" ht="27" customHeight="1">
       <c r="A14">
         <v>12</v>
       </c>
@@ -9264,7 +9807,7 @@
         <v>219F</v>
       </c>
     </row>
-    <row r="15" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:68" ht="27" customHeight="1">
       <c r="A15">
         <v>13</v>
       </c>
@@ -9528,7 +10071,7 @@
         <v>21BF</v>
       </c>
     </row>
-    <row r="16" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:68" ht="27" customHeight="1">
       <c r="A16">
         <v>14</v>
       </c>
@@ -9792,7 +10335,7 @@
         <v>21DF</v>
       </c>
     </row>
-    <row r="17" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:68" ht="27" customHeight="1">
       <c r="A17">
         <v>15</v>
       </c>
@@ -10056,7 +10599,7 @@
         <v>21FF</v>
       </c>
     </row>
-    <row r="18" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:68" ht="27" customHeight="1">
       <c r="A18">
         <v>16</v>
       </c>
@@ -10320,7 +10863,7 @@
         <v>221F</v>
       </c>
     </row>
-    <row r="19" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:68" ht="27" customHeight="1">
       <c r="A19">
         <v>17</v>
       </c>
@@ -10584,7 +11127,7 @@
         <v>223F</v>
       </c>
     </row>
-    <row r="20" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:68" ht="27" customHeight="1">
       <c r="A20">
         <v>18</v>
       </c>
@@ -10848,7 +11391,7 @@
         <v>225F</v>
       </c>
     </row>
-    <row r="21" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:68" ht="27" customHeight="1">
       <c r="A21">
         <v>19</v>
       </c>
@@ -11112,7 +11655,7 @@
         <v>227F</v>
       </c>
     </row>
-    <row r="22" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:68" ht="27" customHeight="1">
       <c r="A22">
         <v>20</v>
       </c>
@@ -11376,7 +11919,7 @@
         <v>229F</v>
       </c>
     </row>
-    <row r="23" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:68" ht="27" customHeight="1">
       <c r="A23">
         <v>21</v>
       </c>
@@ -11640,7 +12183,7 @@
         <v>22BF</v>
       </c>
     </row>
-    <row r="24" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:68" ht="27" customHeight="1">
       <c r="A24">
         <v>22</v>
       </c>
@@ -11904,7 +12447,7 @@
         <v>22DF</v>
       </c>
     </row>
-    <row r="25" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:68" ht="27" customHeight="1">
       <c r="A25">
         <v>23</v>
       </c>
@@ -12168,7 +12711,7 @@
         <v>22FF</v>
       </c>
     </row>
-    <row r="26" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:68" ht="27" customHeight="1">
       <c r="A26">
         <v>24</v>
       </c>
@@ -12432,7 +12975,7 @@
         <v>231F</v>
       </c>
     </row>
-    <row r="27" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:68" ht="27" customHeight="1">
       <c r="A27">
         <v>25</v>
       </c>
@@ -12696,7 +13239,7 @@
         <v>233F</v>
       </c>
     </row>
-    <row r="28" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:68" ht="27" customHeight="1">
       <c r="A28">
         <v>26</v>
       </c>
@@ -12960,7 +13503,7 @@
         <v>235F</v>
       </c>
     </row>
-    <row r="29" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:68" ht="27" customHeight="1">
       <c r="A29">
         <v>27</v>
       </c>
@@ -13224,7 +13767,7 @@
         <v>237F</v>
       </c>
     </row>
-    <row r="30" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:68" ht="27" customHeight="1">
       <c r="A30">
         <v>28</v>
       </c>
@@ -13488,7 +14031,7 @@
         <v>239F</v>
       </c>
     </row>
-    <row r="31" spans="1:68" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:68" ht="27" customHeight="1" thickBot="1">
       <c r="A31">
         <v>29</v>
       </c>
@@ -13760,24 +14303,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD621C5E-94B6-45EE-BBA4-12B279F31EA6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BP31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView topLeftCell="AJ1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AK14" activePane="bottomRight" state="frozenSplit"/>
       <selection activeCell="AJ1" sqref="AJ1"/>
       <selection pane="topRight" activeCell="AK1" sqref="AK1"/>
       <selection pane="bottomLeft" activeCell="AJ2" sqref="AJ2"/>
-      <selection pane="bottomRight" activeCell="AM18" sqref="AM18:BO18"/>
+      <selection pane="bottomRight" activeCell="AL20" sqref="AL20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.875" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="4.85546875" defaultRowHeight="27" customHeight="1"/>
   <cols>
     <col min="1" max="33" width="0" hidden="1" customWidth="1"/>
-    <col min="36" max="68" width="4.875" style="59"/>
+    <col min="36" max="68" width="4.85546875" style="59"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:68" ht="27" customHeight="1" thickBot="1">
       <c r="B1">
         <v>0</v>
       </c>
@@ -13971,7 +14514,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:68" ht="27" customHeight="1">
       <c r="A2">
         <v>0</v>
       </c>
@@ -14110,7 +14653,7 @@
         <v>2000</v>
       </c>
       <c r="AL2" s="67" t="str">
-        <f t="shared" ref="AL2:BA31" si="1">DEC2HEX(8192+C2)</f>
+        <f t="shared" ref="AL2:BA17" si="1">DEC2HEX(8192+C2)</f>
         <v>2001</v>
       </c>
       <c r="AM2" s="67" t="str">
@@ -14174,7 +14717,7 @@
         <v>2010</v>
       </c>
       <c r="BB2" s="67" t="str">
-        <f t="shared" ref="BB2:BP31" si="2">DEC2HEX(8192+S2)</f>
+        <f t="shared" ref="BB2:BP18" si="2">DEC2HEX(8192+S2)</f>
         <v>2011</v>
       </c>
       <c r="BC2" s="67" t="str">
@@ -14234,7 +14777,7 @@
         <v>201F</v>
       </c>
     </row>
-    <row r="3" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:68" ht="27" customHeight="1">
       <c r="A3">
         <v>1</v>
       </c>
@@ -14498,7 +15041,7 @@
         <v>203F</v>
       </c>
     </row>
-    <row r="4" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:68" ht="27" customHeight="1">
       <c r="A4">
         <v>2</v>
       </c>
@@ -14762,7 +15305,7 @@
         <v>205F</v>
       </c>
     </row>
-    <row r="5" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:68" ht="27" customHeight="1">
       <c r="A5">
         <v>3</v>
       </c>
@@ -15026,7 +15569,7 @@
         <v>207F</v>
       </c>
     </row>
-    <row r="6" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:68" ht="27" customHeight="1">
       <c r="A6">
         <v>4</v>
       </c>
@@ -15290,7 +15833,7 @@
         <v>209F</v>
       </c>
     </row>
-    <row r="7" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:68" ht="27" customHeight="1">
       <c r="A7">
         <v>5</v>
       </c>
@@ -15554,7 +16097,7 @@
         <v>20BF</v>
       </c>
     </row>
-    <row r="8" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:68" ht="27" customHeight="1">
       <c r="A8">
         <v>6</v>
       </c>
@@ -15818,7 +16361,7 @@
         <v>20DF</v>
       </c>
     </row>
-    <row r="9" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:68" ht="27" customHeight="1">
       <c r="A9">
         <v>7</v>
       </c>
@@ -16082,7 +16625,7 @@
         <v>20FF</v>
       </c>
     </row>
-    <row r="10" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:68" ht="27" customHeight="1">
       <c r="A10">
         <v>8</v>
       </c>
@@ -16346,7 +16889,7 @@
         <v>211F</v>
       </c>
     </row>
-    <row r="11" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:68" ht="27" customHeight="1">
       <c r="A11">
         <v>9</v>
       </c>
@@ -16610,7 +17153,7 @@
         <v>213F</v>
       </c>
     </row>
-    <row r="12" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:68" ht="27" customHeight="1">
       <c r="A12">
         <v>10</v>
       </c>
@@ -16874,7 +17417,7 @@
         <v>215F</v>
       </c>
     </row>
-    <row r="13" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:68" ht="27" customHeight="1">
       <c r="A13">
         <v>11</v>
       </c>
@@ -17138,7 +17681,7 @@
         <v>217F</v>
       </c>
     </row>
-    <row r="14" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:68" ht="27" customHeight="1">
       <c r="A14">
         <v>12</v>
       </c>
@@ -17402,7 +17945,7 @@
         <v>219F</v>
       </c>
     </row>
-    <row r="15" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:68" ht="27" customHeight="1">
       <c r="A15">
         <v>13</v>
       </c>
@@ -17666,7 +18209,7 @@
         <v>21BF</v>
       </c>
     </row>
-    <row r="16" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:68" ht="27" customHeight="1">
       <c r="A16">
         <v>14</v>
       </c>
@@ -17930,7 +18473,7 @@
         <v>21DF</v>
       </c>
     </row>
-    <row r="17" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:68" ht="27" customHeight="1">
       <c r="A17">
         <v>15</v>
       </c>
@@ -18130,7 +18673,7 @@
         <v>21EF</v>
       </c>
       <c r="BA17" s="61" t="str">
-        <f t="shared" ref="BA17:BP46" si="8">DEC2HEX(8192+R17)</f>
+        <f t="shared" ref="BA17:BP31" si="8">DEC2HEX(8192+R17)</f>
         <v>21F0</v>
       </c>
       <c r="BB17" s="61" t="str">
@@ -18194,7 +18737,7 @@
         <v>21FF</v>
       </c>
     </row>
-    <row r="18" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:68" ht="27" customHeight="1">
       <c r="A18">
         <v>16</v>
       </c>
@@ -18458,7 +19001,7 @@
         <v>221F</v>
       </c>
     </row>
-    <row r="19" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:68" ht="27" customHeight="1">
       <c r="A19">
         <v>17</v>
       </c>
@@ -18722,7 +19265,7 @@
         <v>223F</v>
       </c>
     </row>
-    <row r="20" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:68" ht="27" customHeight="1">
       <c r="A20">
         <v>18</v>
       </c>
@@ -18986,7 +19529,7 @@
         <v>225F</v>
       </c>
     </row>
-    <row r="21" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:68" ht="27" customHeight="1">
       <c r="A21">
         <v>19</v>
       </c>
@@ -19250,7 +19793,7 @@
         <v>227F</v>
       </c>
     </row>
-    <row r="22" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:68" ht="27" customHeight="1">
       <c r="A22">
         <v>20</v>
       </c>
@@ -19514,7 +20057,7 @@
         <v>229F</v>
       </c>
     </row>
-    <row r="23" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:68" ht="27" customHeight="1">
       <c r="A23">
         <v>21</v>
       </c>
@@ -19778,7 +20321,7 @@
         <v>22BF</v>
       </c>
     </row>
-    <row r="24" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:68" ht="27" customHeight="1">
       <c r="A24">
         <v>22</v>
       </c>
@@ -20042,7 +20585,7 @@
         <v>22DF</v>
       </c>
     </row>
-    <row r="25" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:68" ht="27" customHeight="1">
       <c r="A25">
         <v>23</v>
       </c>
@@ -20306,7 +20849,7 @@
         <v>22FF</v>
       </c>
     </row>
-    <row r="26" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:68" ht="27" customHeight="1">
       <c r="A26">
         <v>24</v>
       </c>
@@ -20570,7 +21113,7 @@
         <v>231F</v>
       </c>
     </row>
-    <row r="27" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:68" ht="27" customHeight="1">
       <c r="A27">
         <v>25</v>
       </c>
@@ -20834,7 +21377,7 @@
         <v>233F</v>
       </c>
     </row>
-    <row r="28" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:68" ht="27" customHeight="1">
       <c r="A28">
         <v>26</v>
       </c>
@@ -21098,7 +21641,7 @@
         <v>235F</v>
       </c>
     </row>
-    <row r="29" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:68" ht="27" customHeight="1">
       <c r="A29">
         <v>27</v>
       </c>
@@ -21362,7 +21905,7 @@
         <v>237F</v>
       </c>
     </row>
-    <row r="30" spans="1:68" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:68" ht="27" customHeight="1">
       <c r="A30">
         <v>28</v>
       </c>
@@ -21626,7 +22169,7 @@
         <v>239F</v>
       </c>
     </row>
-    <row r="31" spans="1:68" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:68" ht="27" customHeight="1" thickBot="1">
       <c r="A31">
         <v>29</v>
       </c>
@@ -21898,20 +22441,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Y21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.25" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="5.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="5.25" style="1"/>
+    <col min="1" max="16384" width="5.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:25" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="2:25" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:25" ht="15.75" thickBot="1"/>
+    <row r="3" spans="2:25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -21985,7 +22528,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:25" ht="15.75" thickBot="1">
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
@@ -22059,7 +22602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:25" ht="15.75" thickBot="1">
       <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
@@ -22133,7 +22676,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:25" ht="15.75" thickBot="1">
       <c r="B6" s="11" t="s">
         <v>10</v>
       </c>
@@ -22207,7 +22750,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:25" ht="15.75" thickBot="1">
       <c r="B7" s="8" t="s">
         <v>17</v>
       </c>
@@ -22281,7 +22824,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:25" ht="15.75" thickBot="1">
       <c r="B8" s="11" t="s">
         <v>24</v>
       </c>
@@ -22355,7 +22898,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:25" ht="15.75" thickBot="1">
       <c r="B9" s="8" t="s">
         <v>31</v>
       </c>
@@ -22429,7 +22972,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:25" ht="15.75" thickBot="1">
       <c r="B10" s="11" t="s">
         <v>38</v>
       </c>
@@ -22503,7 +23046,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:25" ht="15.75" thickBot="1">
       <c r="B11" s="8" t="s">
         <v>45</v>
       </c>
@@ -22577,7 +23120,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:25" ht="15.75" thickBot="1">
       <c r="B12" s="11" t="s">
         <v>52</v>
       </c>
@@ -22651,7 +23194,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:25" ht="15.75" thickBot="1">
       <c r="B13" s="8" t="s">
         <v>59</v>
       </c>
@@ -22725,7 +23268,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:25" ht="15.75" thickBot="1">
       <c r="B14" s="11" t="s">
         <v>66</v>
       </c>
@@ -22799,7 +23342,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:25" ht="15.75" thickBot="1">
       <c r="B15" s="8" t="s">
         <v>73</v>
       </c>
@@ -22873,7 +23416,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:25" ht="15.75" thickBot="1">
       <c r="B16" s="11" t="s">
         <v>89</v>
       </c>
@@ -22947,7 +23490,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:25" ht="15.75" thickBot="1">
       <c r="B17" s="8" t="s">
         <v>105</v>
       </c>
@@ -23021,7 +23564,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:25" ht="15.75" thickBot="1">
       <c r="B18" s="11" t="s">
         <v>121</v>
       </c>
@@ -23095,7 +23638,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:25" ht="15.75" thickBot="1">
       <c r="B19" s="8" t="s">
         <v>137</v>
       </c>
@@ -23169,7 +23712,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:25" ht="15.75" thickBot="1">
       <c r="B20" s="30" t="s">
         <v>153</v>
       </c>
@@ -23243,7 +23786,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="21" spans="2:25" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:25">
       <c r="B21" s="45" t="s">
         <v>169</v>
       </c>
@@ -23255,27 +23798,48 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="O27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AB24" sqref="AB24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="27" spans="15:15">
+      <c r="O27" t="s">
+        <v>297</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C113"/>
   <sheetViews>
     <sheetView topLeftCell="A89" workbookViewId="0">
       <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="59.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="42.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="64.25" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.125" style="1"/>
+    <col min="1" max="1" width="59.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="64.28515625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1">
       <c r="A2" s="46" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
       <c r="A3" s="47" t="s">
         <v>171</v>
       </c>
@@ -23283,12 +23847,12 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15.75" thickBot="1">
       <c r="A4" s="48" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="15.75" thickBot="1">
       <c r="A5" s="49" t="s">
         <v>174</v>
       </c>
@@ -23299,7 +23863,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15.75" thickBot="1">
       <c r="A6" s="49" t="s">
         <v>177</v>
       </c>
@@ -23310,7 +23874,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15.75" thickBot="1">
       <c r="A7" s="49" t="s">
         <v>180</v>
       </c>
@@ -23321,25 +23885,25 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A8" s="83" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="81" t="s">
         <v>183</v>
       </c>
-      <c r="B8" s="83" t="s">
+      <c r="B8" s="81" t="s">
         <v>184</v>
       </c>
       <c r="C8" s="50" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="84"/>
-      <c r="B9" s="84"/>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A9" s="82"/>
+      <c r="B9" s="82"/>
       <c r="C9" s="51" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="15.75" thickBot="1">
       <c r="A10" s="49" t="s">
         <v>187</v>
       </c>
@@ -23350,7 +23914,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="29.25" thickBot="1">
       <c r="A11" s="49" t="s">
         <v>190</v>
       </c>
@@ -23361,7 +23925,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="15.75" thickBot="1">
       <c r="A12" s="49" t="s">
         <v>192</v>
       </c>
@@ -23372,25 +23936,25 @@
         <v>194</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A13" s="83" t="s">
+    <row r="13" spans="1:3">
+      <c r="A13" s="81" t="s">
         <v>195</v>
       </c>
-      <c r="B13" s="83" t="s">
+      <c r="B13" s="81" t="s">
         <v>196</v>
       </c>
       <c r="C13" s="50" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="84"/>
-      <c r="B14" s="84"/>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A14" s="82"/>
+      <c r="B14" s="82"/>
       <c r="C14" s="51" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="15.75" thickBot="1">
       <c r="A15" s="47" t="s">
         <v>199</v>
       </c>
@@ -23398,12 +23962,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15.75" thickBot="1">
       <c r="A16" s="48" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="15.75" thickBot="1">
       <c r="A17" s="49" t="s">
         <v>174</v>
       </c>
@@ -23414,7 +23978,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15.75" thickBot="1">
       <c r="A18" s="49" t="s">
         <v>177</v>
       </c>
@@ -23425,7 +23989,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15.75" thickBot="1">
       <c r="A19" s="49" t="s">
         <v>180</v>
       </c>
@@ -23436,7 +24000,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15.75" thickBot="1">
       <c r="A20" s="49" t="s">
         <v>183</v>
       </c>
@@ -23447,7 +24011,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15.75" thickBot="1">
       <c r="A21" s="49" t="s">
         <v>187</v>
       </c>
@@ -23458,7 +24022,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="15.75" thickBot="1">
       <c r="A22" s="49" t="s">
         <v>190</v>
       </c>
@@ -23469,7 +24033,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="29.25" thickBot="1">
       <c r="A23" s="49" t="s">
         <v>192</v>
       </c>
@@ -23480,7 +24044,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="15.75" thickBot="1">
       <c r="A24" s="49" t="s">
         <v>209</v>
       </c>
@@ -23491,7 +24055,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="15.75" thickBot="1">
       <c r="A25" s="49" t="s">
         <v>211</v>
       </c>
@@ -23502,17 +24066,17 @@
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="15.75" thickBot="1">
       <c r="A26" s="47" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="15.75" thickBot="1">
       <c r="A27" s="48" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15.75" thickBot="1">
       <c r="A28" s="49" t="s">
         <v>174</v>
       </c>
@@ -23523,25 +24087,25 @@
         <v>176</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A29" s="83" t="s">
+    <row r="29" spans="1:3">
+      <c r="A29" s="81" t="s">
         <v>177</v>
       </c>
-      <c r="B29" s="83" t="s">
+      <c r="B29" s="81" t="s">
         <v>216</v>
       </c>
       <c r="C29" s="50" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="84"/>
-      <c r="B30" s="84"/>
+    <row r="30" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A30" s="82"/>
+      <c r="B30" s="82"/>
       <c r="C30" s="51" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="29.25" thickBot="1">
       <c r="A31" s="49" t="s">
         <v>180</v>
       </c>
@@ -23552,7 +24116,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="29.25" thickBot="1">
       <c r="A32" s="49" t="s">
         <v>183</v>
       </c>
@@ -23563,25 +24127,25 @@
         <v>222</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A33" s="83" t="s">
+    <row r="33" spans="1:3">
+      <c r="A33" s="81" t="s">
         <v>187</v>
       </c>
-      <c r="B33" s="83" t="s">
+      <c r="B33" s="81" t="s">
         <v>223</v>
       </c>
       <c r="C33" s="50" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="84"/>
-      <c r="B34" s="84"/>
+    <row r="34" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A34" s="82"/>
+      <c r="B34" s="82"/>
       <c r="C34" s="51" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="15.75" thickBot="1">
       <c r="A35" s="49" t="s">
         <v>226</v>
       </c>
@@ -23590,17 +24154,17 @@
       </c>
       <c r="C35" s="49"/>
     </row>
-    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="15.75" thickBot="1">
       <c r="A36" s="47" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="15.75" thickBot="1">
       <c r="A37" s="48" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="15.75" thickBot="1">
       <c r="A38" s="49" t="s">
         <v>174</v>
       </c>
@@ -23611,7 +24175,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="15.75" thickBot="1">
       <c r="A39" s="49" t="s">
         <v>230</v>
       </c>
@@ -23622,17 +24186,17 @@
         <v>232</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="15.75" thickBot="1">
       <c r="A40" s="47" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="15.75" thickBot="1">
       <c r="A41" s="48" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="15.75" thickBot="1">
       <c r="A42" s="49" t="s">
         <v>174</v>
       </c>
@@ -23643,7 +24207,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="15.75" thickBot="1">
       <c r="A43" s="49" t="s">
         <v>230</v>
       </c>
@@ -23654,17 +24218,17 @@
         <v>232</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="15.75" thickBot="1">
       <c r="A44" s="47" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="39" thickBot="1">
       <c r="A45" s="48" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" ht="15.75" thickBot="1">
       <c r="A46" s="49" t="s">
         <v>174</v>
       </c>
@@ -23675,35 +24239,35 @@
         <v>176</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A47" s="83" t="s">
+    <row r="47" spans="1:3">
+      <c r="A47" s="81" t="s">
         <v>230</v>
       </c>
       <c r="B47" s="50" t="s">
         <v>238</v>
       </c>
-      <c r="C47" s="83" t="s">
+      <c r="C47" s="81" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="84"/>
+    <row r="48" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A48" s="82"/>
       <c r="B48" s="51" t="s">
         <v>239</v>
       </c>
-      <c r="C48" s="84"/>
+      <c r="C48" s="82"/>
     </row>
-    <row r="49" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="15.75" thickBot="1">
       <c r="A49" s="47" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="39" thickBot="1">
       <c r="A50" s="48" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="15.75" thickBot="1">
       <c r="A51" s="49" t="s">
         <v>174</v>
       </c>
@@ -23714,35 +24278,35 @@
         <v>176</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A52" s="83" t="s">
+    <row r="52" spans="1:3">
+      <c r="A52" s="81" t="s">
         <v>230</v>
       </c>
       <c r="B52" s="50" t="s">
         <v>242</v>
       </c>
-      <c r="C52" s="83" t="s">
+      <c r="C52" s="81" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="84"/>
+    <row r="53" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A53" s="82"/>
       <c r="B53" s="51" t="s">
         <v>243</v>
       </c>
-      <c r="C53" s="84"/>
+      <c r="C53" s="82"/>
     </row>
-    <row r="54" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" ht="15.75" thickBot="1">
       <c r="A54" s="47" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" ht="26.25" thickBot="1">
       <c r="A55" s="48" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" ht="15.75" thickBot="1">
       <c r="A56" s="49" t="s">
         <v>174</v>
       </c>
@@ -23753,39 +24317,39 @@
         <v>176</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A57" s="83" t="s">
+    <row r="57" spans="1:3">
+      <c r="A57" s="81" t="s">
         <v>230</v>
       </c>
       <c r="B57" s="50" t="s">
         <v>246</v>
       </c>
-      <c r="C57" s="83" t="s">
+      <c r="C57" s="81" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="84"/>
+    <row r="58" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A58" s="82"/>
       <c r="B58" s="51" t="s">
         <v>247</v>
       </c>
-      <c r="C58" s="84"/>
+      <c r="C58" s="82"/>
     </row>
-    <row r="62" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="15.75" thickBot="1">
       <c r="A62" s="69" t="s">
         <v>254</v>
       </c>
       <c r="B62"/>
       <c r="C62"/>
     </row>
-    <row r="63" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="39.75" thickBot="1">
       <c r="A63" s="70" t="s">
         <v>255</v>
       </c>
       <c r="B63"/>
       <c r="C63"/>
     </row>
-    <row r="64" spans="1:3" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="15.75" thickBot="1">
       <c r="A64" s="71" t="s">
         <v>174</v>
       </c>
@@ -23796,7 +24360,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="15.75" thickBot="1">
       <c r="A65" s="71" t="s">
         <v>230</v>
       </c>
@@ -23807,21 +24371,21 @@
         <v>257</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="15.75" thickBot="1">
       <c r="A70" s="69" t="s">
         <v>258</v>
       </c>
       <c r="B70"/>
       <c r="C70"/>
     </row>
-    <row r="71" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="39.75" thickBot="1">
       <c r="A71" s="70" t="s">
         <v>259</v>
       </c>
       <c r="B71"/>
       <c r="C71"/>
     </row>
-    <row r="72" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="15.75" thickBot="1">
       <c r="A72" s="72" t="s">
         <v>174</v>
       </c>
@@ -23832,7 +24396,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="15.75" thickBot="1">
       <c r="A73" s="72" t="s">
         <v>260</v>
       </c>
@@ -23841,8 +24405,8 @@
       </c>
       <c r="C73" s="72"/>
     </row>
-    <row r="74" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A74" s="81" t="s">
+    <row r="74" spans="1:3">
+      <c r="A74" s="83" t="s">
         <v>187</v>
       </c>
       <c r="B74" s="73" t="s">
@@ -23852,8 +24416,8 @@
         <v>263</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="82"/>
+    <row r="75" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A75" s="84"/>
       <c r="B75" s="74" t="s">
         <v>262</v>
       </c>
@@ -23861,44 +24425,44 @@
         <v>264</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A76" s="81" t="s">
+    <row r="76" spans="1:3">
+      <c r="A76" s="83" t="s">
         <v>190</v>
       </c>
       <c r="B76" s="73" t="s">
         <v>265</v>
       </c>
-      <c r="C76" s="81" t="s">
+      <c r="C76" s="83" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="82"/>
+    <row r="77" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A77" s="84"/>
       <c r="B77" s="74" t="s">
         <v>262</v>
       </c>
-      <c r="C77" s="82"/>
+      <c r="C77" s="84"/>
     </row>
-    <row r="78" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A78" s="81" t="s">
+    <row r="78" spans="1:3">
+      <c r="A78" s="83" t="s">
         <v>267</v>
       </c>
       <c r="B78" s="73" t="s">
         <v>268</v>
       </c>
-      <c r="C78" s="81" t="s">
+      <c r="C78" s="83" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="82"/>
+    <row r="79" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A79" s="84"/>
       <c r="B79" s="74" t="s">
         <v>269</v>
       </c>
-      <c r="C79" s="82"/>
+      <c r="C79" s="84"/>
     </row>
-    <row r="80" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A80" s="81" t="s">
+    <row r="80" spans="1:3">
+      <c r="A80" s="83" t="s">
         <v>211</v>
       </c>
       <c r="B80" s="73" t="s">
@@ -23908,8 +24472,8 @@
         <v>272</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="82"/>
+    <row r="81" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A81" s="84"/>
       <c r="B81" s="74" t="s">
         <v>271</v>
       </c>
@@ -23917,21 +24481,21 @@
         <v>273</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" ht="15.75" thickBot="1">
       <c r="A82" s="69" t="s">
         <v>274</v>
       </c>
       <c r="B82"/>
       <c r="C82"/>
     </row>
-    <row r="83" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="15.75" thickBot="1">
       <c r="A83" s="70" t="s">
         <v>275</v>
       </c>
       <c r="B83"/>
       <c r="C83"/>
     </row>
-    <row r="84" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" ht="15.75" thickBot="1">
       <c r="A84" s="72" t="s">
         <v>174</v>
       </c>
@@ -23942,7 +24506,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" ht="15.75" thickBot="1">
       <c r="A85" s="72" t="s">
         <v>260</v>
       </c>
@@ -23951,25 +24515,25 @@
       </c>
       <c r="C85" s="72"/>
     </row>
-    <row r="86" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A86" s="81" t="s">
+    <row r="86" spans="1:3">
+      <c r="A86" s="83" t="s">
         <v>187</v>
       </c>
-      <c r="B86" s="81" t="s">
+      <c r="B86" s="83" t="s">
         <v>276</v>
       </c>
       <c r="C86" s="73" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="82"/>
-      <c r="B87" s="82"/>
+    <row r="87" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A87" s="84"/>
+      <c r="B87" s="84"/>
       <c r="C87" s="74" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="15.75" thickBot="1">
       <c r="A88" s="72" t="s">
         <v>190</v>
       </c>
@@ -23980,7 +24544,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="15.75" thickBot="1">
       <c r="A89" s="72" t="s">
         <v>267</v>
       </c>
@@ -23991,7 +24555,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="15.75" thickBot="1">
       <c r="A90" s="72" t="s">
         <v>211</v>
       </c>
@@ -24002,55 +24566,55 @@
         <v>266</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" ht="15.75" thickBot="1">
       <c r="A94" s="69" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3">
       <c r="A95" s="70" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3">
       <c r="A96" s="76" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2">
       <c r="A97" s="76" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" ht="38.25">
       <c r="A98" s="76" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" ht="38.25">
       <c r="A99" s="76" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" ht="16.5" thickBot="1">
       <c r="A102" s="75" t="s">
         <v>280</v>
       </c>
       <c r="B102"/>
     </row>
-    <row r="103" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
       <c r="A103" s="69" t="s">
         <v>281</v>
       </c>
       <c r="B103"/>
     </row>
-    <row r="104" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" ht="52.5" thickBot="1">
       <c r="A104" s="70" t="s">
         <v>282</v>
       </c>
       <c r="B104"/>
     </row>
-    <row r="105" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" ht="15.75" thickBot="1">
       <c r="A105" s="72" t="s">
         <v>283</v>
       </c>
@@ -24058,7 +24622,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" ht="15.75" thickBot="1">
       <c r="A106" s="72">
         <v>1</v>
       </c>
@@ -24066,7 +24630,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" ht="15.75" thickBot="1">
       <c r="A107" s="72">
         <v>2</v>
       </c>
@@ -24074,7 +24638,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" ht="15.75" thickBot="1">
       <c r="A108" s="72">
         <v>3</v>
       </c>
@@ -24082,7 +24646,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" ht="15.75" thickBot="1">
       <c r="A109" s="72">
         <v>4</v>
       </c>
@@ -24090,7 +24654,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" ht="15.75" thickBot="1">
       <c r="A110" s="72">
         <v>5</v>
       </c>
@@ -24098,7 +24662,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" ht="15.75" thickBot="1">
       <c r="A111" s="72">
         <v>6</v>
       </c>
@@ -24106,7 +24670,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" ht="15.75" thickBot="1">
       <c r="A112" s="72">
         <v>7</v>
       </c>
@@ -24114,7 +24678,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" ht="15.75" thickBot="1">
       <c r="A113" s="72">
         <v>8</v>
       </c>
@@ -24124,28 +24688,28 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="C52:C53"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="B29:B30"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="A76:A77"/>
   </mergeCells>
   <phoneticPr fontId="12"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>